<commit_message>
Se arreglaron errores con las acciones de administrador para modificar y agregar usuarios, se avanzo en funcionalidades de instructor para generar asistencias
</commit_message>
<xml_diff>
--- a/Proyecto_Registro_Asistencia/asistencia.xlsx
+++ b/Proyecto_Registro_Asistencia/asistencia.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Nombres</t>
   </si>
@@ -41,6 +41,33 @@
     <t>Estado</t>
   </si>
   <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>Cedula de Ciudadania</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>No Aplica</t>
+  </si>
+  <si>
+    <t>Algoritmia</t>
+  </si>
+  <si>
+    <t>08:45 a. m.</t>
+  </si>
+  <si>
+    <t>A tiempo</t>
+  </si>
+  <si>
     <t>Jeisson Fernando</t>
   </si>
   <si>
@@ -53,19 +80,22 @@
     <t>1097096255</t>
   </si>
   <si>
-    <t>No aplica</t>
-  </si>
-  <si>
     <t>Tecnologo</t>
   </si>
   <si>
-    <t>Algoritmia</t>
-  </si>
-  <si>
-    <t>04:25 p. m.</t>
-  </si>
-  <si>
-    <t>Tarde</t>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>alfonso</t>
+  </si>
+  <si>
+    <t>Tarjeta de Extranjeria</t>
+  </si>
+  <si>
+    <t>987654321</t>
+  </si>
+  <si>
+    <t>Electricidad</t>
   </si>
 </sst>
 </file>
@@ -110,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -176,22 +206,22 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>13</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>15</v>
@@ -200,6 +230,35 @@
         <v>16</v>
       </c>
       <c r="I3" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s" s="0">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se completo la funcionalidad de generar excel, subirlos a la base de datos y de listarlos en la pantalla de inicio del instructor, se completo la funcionalidad de registro de aprendiz cuando no cuenta con usuario
</commit_message>
<xml_diff>
--- a/Proyecto_Registro_Asistencia/asistencia.xlsx
+++ b/Proyecto_Registro_Asistencia/asistencia.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Nombres</t>
   </si>
@@ -41,6 +41,33 @@
     <t>Estado</t>
   </si>
   <si>
+    <t>pablo</t>
+  </si>
+  <si>
+    <t>alfonso</t>
+  </si>
+  <si>
+    <t>Tarjeta de Extranjeria</t>
+  </si>
+  <si>
+    <t>987321654</t>
+  </si>
+  <si>
+    <t>ADSO</t>
+  </si>
+  <si>
+    <t>Tecnologo</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>05:35 p. m.</t>
+  </si>
+  <si>
+    <t>A tiempo</t>
+  </si>
+  <si>
     <t>Juan</t>
   </si>
   <si>
@@ -59,13 +86,7 @@
     <t>No Aplica</t>
   </si>
   <si>
-    <t>Algoritmia</t>
-  </si>
-  <si>
-    <t>08:45 a. m.</t>
-  </si>
-  <si>
-    <t>A tiempo</t>
+    <t>05:36 p. m.</t>
   </si>
   <si>
     <t>Jeisson Fernando</t>
@@ -80,16 +101,7 @@
     <t>1097096255</t>
   </si>
   <si>
-    <t>Tecnologo</t>
-  </si>
-  <si>
     <t>juan</t>
-  </si>
-  <si>
-    <t>alfonso</t>
-  </si>
-  <si>
-    <t>Tarjeta de Extranjeria</t>
   </si>
   <si>
     <t>987654321</t>
@@ -140,7 +152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -218,16 +230,16 @@
         <v>21</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>15</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s" s="0">
         <v>17</v>
@@ -235,30 +247,59 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>15</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s" s="0">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se completo la caracteristica de establecer y usar las credenciales de usuario de manera global
</commit_message>
<xml_diff>
--- a/Proyecto_Registro_Asistencia/asistencia.xlsx
+++ b/Proyecto_Registro_Asistencia/asistencia.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Nombres</t>
   </si>
@@ -41,67 +41,37 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>pablo</t>
+    <t>Jeisson</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>Cedula de Extranjeria</t>
+  </si>
+  <si>
+    <t>1097096255</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>Tecnologo</t>
+  </si>
+  <si>
+    <t>ciber seguridad</t>
+  </si>
+  <si>
+    <t>08:14 p. m.</t>
+  </si>
+  <si>
+    <t>A tiempo</t>
+  </si>
+  <si>
+    <t>juan</t>
   </si>
   <si>
     <t>alfonso</t>
-  </si>
-  <si>
-    <t>Tarjeta de Extranjeria</t>
-  </si>
-  <si>
-    <t>987321654</t>
-  </si>
-  <si>
-    <t>ADSO</t>
-  </si>
-  <si>
-    <t>Tecnologo</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>05:35 p. m.</t>
-  </si>
-  <si>
-    <t>A tiempo</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Pablo</t>
-  </si>
-  <si>
-    <t>Cedula de Ciudadania</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>No aplica</t>
-  </si>
-  <si>
-    <t>No Aplica</t>
-  </si>
-  <si>
-    <t>05:36 p. m.</t>
-  </si>
-  <si>
-    <t>Jeisson Fernando</t>
-  </si>
-  <si>
-    <t>Leon Avila</t>
-  </si>
-  <si>
-    <t>Cedula de Extranjeria</t>
-  </si>
-  <si>
-    <t>1097096255</t>
-  </si>
-  <si>
-    <t>juan</t>
   </si>
   <si>
     <t>987654321</t>
@@ -152,7 +122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -224,82 +194,24 @@
         <v>19</v>
       </c>
       <c r="C3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E3" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="E3" t="s" s="0">
-        <v>22</v>
-      </c>
       <c r="F3" t="s" s="0">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>15</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="I5" t="s" s="0">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se hicieron cambios en la base de datos, se completo la funcionalidad de registrar las horas de inasistencia por fichas, cambios minimos en funciones generales
</commit_message>
<xml_diff>
--- a/Proyecto_Registro_Asistencia/asistencia.xlsx
+++ b/Proyecto_Registro_Asistencia/asistencia.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Nombres</t>
   </si>
@@ -59,13 +59,28 @@
     <t>Tecnologo</t>
   </si>
   <si>
-    <t>ciber</t>
-  </si>
-  <si>
-    <t>03:40 p. m.</t>
-  </si>
-  <si>
-    <t>Tarde</t>
+    <t/>
+  </si>
+  <si>
+    <t>10:52 a. m.</t>
+  </si>
+  <si>
+    <t>A tiempo</t>
+  </si>
+  <si>
+    <t>Victor Manuel</t>
+  </si>
+  <si>
+    <t>Bonilla Gutierrez</t>
+  </si>
+  <si>
+    <t>Permiso por Protección Temporal</t>
+  </si>
+  <si>
+    <t>4073477</t>
+  </si>
+  <si>
+    <t>ADSO</t>
   </si>
 </sst>
 </file>
@@ -133,7 +148,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -197,8 +212,37 @@
         <v>17</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" operator="equal" dxfId="0" priority="1">
       <formula>"A tiempo"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Se completaron los endpoints de historicos y se hicieron arreglos grandes tanto en la base de datos, API y aplicativo de escritorio
</commit_message>
<xml_diff>
--- a/Proyecto_Registro_Asistencia/asistencia.xlsx
+++ b/Proyecto_Registro_Asistencia/asistencia.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Nombres</t>
   </si>
@@ -47,7 +47,7 @@
     <t>Leon</t>
   </si>
   <si>
-    <t>Cedula de Extranjeria</t>
+    <t>Cedula de Ciudadania</t>
   </si>
   <si>
     <t>1097096255</t>
@@ -59,28 +59,13 @@
     <t>Tecnologo</t>
   </si>
   <si>
-    <t/>
+    <t>Algoritmia</t>
   </si>
   <si>
-    <t>10:52 a. m.</t>
+    <t>04:21 p. m.</t>
   </si>
   <si>
     <t>A tiempo</t>
-  </si>
-  <si>
-    <t>Victor Manuel</t>
-  </si>
-  <si>
-    <t>Bonilla Gutierrez</t>
-  </si>
-  <si>
-    <t>Permiso por Protección Temporal</t>
-  </si>
-  <si>
-    <t>4073477</t>
-  </si>
-  <si>
-    <t>ADSO</t>
   </si>
 </sst>
 </file>
@@ -120,35 +105,12 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF4747"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -212,47 +174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I3">
-    <cfRule type="cellIs" operator="equal" dxfId="0" priority="1">
-      <formula>"A tiempo"</formula>
-    </cfRule>
-    <cfRule type="cellIs" operator="equal" dxfId="1" priority="2">
-      <formula>"Tarde"</formula>
-    </cfRule>
-    <cfRule type="cellIs" operator="equal" dxfId="2" priority="3">
-      <formula>"Inasistencia"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se arreglaron varios archivos de consultas a la API
</commit_message>
<xml_diff>
--- a/Proyecto_Registro_Asistencia/asistencia.xlsx
+++ b/Proyecto_Registro_Asistencia/asistencia.xlsx
@@ -41,28 +41,28 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>Jeisson</t>
+    <t>Victor Manuel</t>
   </si>
   <si>
-    <t>Leon</t>
+    <t>Bonilla Gutierrez</t>
   </si>
   <si>
-    <t>Cedula de Ciudadania</t>
+    <t>Permiso por Protección Temporal</t>
   </si>
   <si>
-    <t>1097096255</t>
+    <t>4073477</t>
   </si>
   <si>
-    <t>No aplica</t>
+    <t>ADSO</t>
   </si>
   <si>
     <t>Tecnologo</t>
   </si>
   <si>
-    <t>Algoritmia</t>
+    <t>Desarrollo Web</t>
   </si>
   <si>
-    <t>04:21 p. m.</t>
+    <t>03:34 p. m.</t>
   </si>
   <si>
     <t>A tiempo</t>

</xml_diff>